<commit_message>
weekly data processing added
</commit_message>
<xml_diff>
--- a/google-trends/output/period_data.xlsx
+++ b/google-trends/output/period_data.xlsx
@@ -14,12 +14,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+  <si>
+    <t>period_name</t>
+  </si>
   <si>
     <t>CZK</t>
   </si>
   <si>
     <t>česká koruna</t>
+  </si>
+  <si>
+    <t>2004q1</t>
+  </si>
+  <si>
+    <t>2004q2</t>
+  </si>
+  <si>
+    <t>2004q3</t>
+  </si>
+  <si>
+    <t>2004q4</t>
+  </si>
+  <si>
+    <t>2005q1</t>
+  </si>
+  <si>
+    <t>2005q2</t>
+  </si>
+  <si>
+    <t>2005q3</t>
+  </si>
+  <si>
+    <t>2005q4</t>
+  </si>
+  <si>
+    <t>2006q1</t>
+  </si>
+  <si>
+    <t>2006q2</t>
+  </si>
+  <si>
+    <t>2006q3</t>
+  </si>
+  <si>
+    <t>2006q4</t>
+  </si>
+  <si>
+    <t>2007q1</t>
+  </si>
+  <si>
+    <t>2007q2</t>
+  </si>
+  <si>
+    <t>2007q3</t>
+  </si>
+  <si>
+    <t>2007q4</t>
+  </si>
+  <si>
+    <t>2008q1</t>
+  </si>
+  <si>
+    <t>2008q2</t>
+  </si>
+  <si>
+    <t>2008q3</t>
+  </si>
+  <si>
+    <t>2008q4</t>
+  </si>
+  <si>
+    <t>2009q1</t>
+  </si>
+  <si>
+    <t>2009q2</t>
+  </si>
+  <si>
+    <t>2009q3</t>
+  </si>
+  <si>
+    <t>2009q4</t>
+  </si>
+  <si>
+    <t>2010q1</t>
+  </si>
+  <si>
+    <t>2010q2</t>
+  </si>
+  <si>
+    <t>2010q3</t>
+  </si>
+  <si>
+    <t>2010q4</t>
+  </si>
+  <si>
+    <t>2011q1</t>
+  </si>
+  <si>
+    <t>2011q2</t>
+  </si>
+  <si>
+    <t>2011q3</t>
+  </si>
+  <si>
+    <t>2011q4</t>
+  </si>
+  <si>
+    <t>2012q1</t>
+  </si>
+  <si>
+    <t>2012q2</t>
+  </si>
+  <si>
+    <t>2012q3</t>
+  </si>
+  <si>
+    <t>2012q4</t>
+  </si>
+  <si>
+    <t>2013q1</t>
+  </si>
+  <si>
+    <t>2013q2</t>
+  </si>
+  <si>
+    <t>2013q3</t>
+  </si>
+  <si>
+    <t>2013q4</t>
+  </si>
+  <si>
+    <t>2014q1</t>
+  </si>
+  <si>
+    <t>2014q2</t>
+  </si>
+  <si>
+    <t>2014q3</t>
+  </si>
+  <si>
+    <t>2014q4</t>
+  </si>
+  <si>
+    <t>2015q1</t>
+  </si>
+  <si>
+    <t>2015q2</t>
+  </si>
+  <si>
+    <t>2015q3</t>
   </si>
 </sst>
 </file>
@@ -356,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -365,6 +509,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
       <c r="B1" t="n">
         <v>1</v>
       </c>
@@ -373,244 +520,529 @@
       </c>
     </row>
     <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3.076923076923077</v>
+      </c>
       <c r="C3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.846153846153846</v>
+      </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>21.76923076923077</v>
+      </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="n">
+        <v>21.30769230769231</v>
+      </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
+        <v>25.38461538461538</v>
+      </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>25.53846153846154</v>
+      </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>30.07692307692308</v>
+      </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="n">
+        <v>37.53846153846154</v>
+      </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="n">
+        <v>43.61538461538461</v>
+      </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="n">
+        <v>37.15384615384615</v>
+      </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="n">
+        <v>39.15384615384615</v>
+      </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="n">
+        <v>37.46153846153846</v>
+      </c>
       <c r="C24" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="n">
+        <v>44.69230769230769</v>
+      </c>
       <c r="C25" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="n">
+        <v>44.15384615384615</v>
+      </c>
       <c r="C26" t="n">
-        <v>47</v>
+        <v>47.66666666666666</v>
       </c>
     </row>
     <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="n">
+        <v>46.61538461538461</v>
+      </c>
       <c r="C27" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="n">
+        <v>47.69230769230769</v>
+      </c>
       <c r="C28" t="n">
-        <v>61</v>
+        <v>61.33333333333334</v>
       </c>
     </row>
     <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="n">
+        <v>49.53846153846154</v>
+      </c>
       <c r="C29" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="n">
+        <v>45.61538461538461</v>
+      </c>
       <c r="C30" t="n">
-        <v>38</v>
+        <v>38.66666666666666</v>
       </c>
     </row>
     <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="n">
+        <v>42.38461538461539</v>
+      </c>
       <c r="C31" t="n">
-        <v>29</v>
+        <v>29.33333333333333</v>
       </c>
     </row>
     <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="n">
+        <v>46.23076923076923</v>
+      </c>
       <c r="C32" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="n">
+        <v>51.84615384615385</v>
+      </c>
       <c r="C33" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="n">
+        <v>47.61538461538461</v>
+      </c>
       <c r="C34" t="n">
-        <v>27</v>
+        <v>27.66666666666667</v>
       </c>
     </row>
     <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="n">
+        <v>41.53846153846154</v>
+      </c>
       <c r="C35" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="n">
+        <v>45.15384615384615</v>
+      </c>
       <c r="C36" t="n">
-        <v>25</v>
+        <v>25.33333333333333</v>
       </c>
     </row>
     <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="n">
+        <v>53</v>
+      </c>
       <c r="C37" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="n">
+        <v>45.15384615384615</v>
+      </c>
       <c r="C38" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="n">
+        <v>45</v>
+      </c>
       <c r="C39" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="n">
+        <v>47.38461538461539</v>
+      </c>
       <c r="C40" t="n">
-        <v>21</v>
+        <v>21.66666666666667</v>
       </c>
     </row>
     <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="n">
+        <v>59.23076923076923</v>
+      </c>
       <c r="C41" t="n">
         <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="n">
+        <v>57.84615384615385</v>
+      </c>
       <c r="C42" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="n">
+        <v>58.07692307692308</v>
+      </c>
       <c r="C43" t="n">
-        <v>24</v>
+        <v>24.33333333333333</v>
       </c>
     </row>
     <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="n">
+        <v>59.53846153846154</v>
+      </c>
       <c r="C44" t="n">
-        <v>26</v>
+        <v>26.66666666666667</v>
       </c>
     </row>
     <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="n">
+        <v>69.92307692307692</v>
+      </c>
       <c r="C45" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="n">
+        <v>68.15384615384616</v>
+      </c>
       <c r="C46" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="n">
+        <v>77.69230769230769</v>
+      </c>
       <c r="C47" t="n">
-        <v>25</v>
+        <v>25.66666666666667</v>
       </c>
     </row>
     <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="n">
+        <v>80.07692307692308</v>
+      </c>
       <c r="C48" t="n">
-        <v>22</v>
+        <v>22.33333333333333</v>
       </c>
     </row>
     <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="n">
+        <v>94.53846153846153</v>
+      </c>
       <c r="C49" t="n">
         <v>24</v>
       </c>

</xml_diff>